<commit_message>
update figures and readme
</commit_message>
<xml_diff>
--- a/docs/functions_and_arguments.xlsx
+++ b/docs/functions_and_arguments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\proj\ROAD\road\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2132551-3E10-4FF5-9398-9A0E3B42262F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B34A6FE-5CAF-4A5A-A0EB-51D7FE5BD6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="94">
   <si>
     <t>road_get_localities()</t>
   </si>
@@ -416,12 +416,18 @@
   <si>
     <t>road_get_publications()</t>
   </si>
+  <si>
+    <t>LOD 2</t>
+  </si>
+  <si>
+    <t>LOD 3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -489,6 +495,19 @@
       <name val="Aptos"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -498,7 +517,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -506,11 +525,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -531,18 +565,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -550,6 +572,50 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -835,26 +901,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA191576-E575-4853-A1BC-43BBBFBC35B4}">
-  <dimension ref="A1:AC17"/>
+  <dimension ref="A1:AD17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD17" sqref="A1:AD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
-    <col min="3" max="29" width="3.7109375" customWidth="1"/>
+    <col min="1" max="2" width="3.7265625" customWidth="1"/>
+    <col min="3" max="3" width="33.1796875" customWidth="1"/>
+    <col min="4" max="30" width="3.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="12" t="s">
+    <row r="1" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="12"/>
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
@@ -862,906 +930,10 @@
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="12"/>
+      <c r="M1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-    </row>
-    <row r="2" spans="1:29" ht="166.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="6"/>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" s="9"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6"/>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="9"/>
-      <c r="M6" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="6"/>
-      <c r="AA6" s="6"/>
-      <c r="AB6" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="6"/>
-      <c r="AB7" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="6"/>
-      <c r="AB8" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="6"/>
-      <c r="AB9" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="6"/>
-      <c r="AB10" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="T11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
-      <c r="AA11" s="6"/>
-      <c r="AB11" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="V12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="W12" s="6"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="6"/>
-      <c r="AA12" s="6"/>
-      <c r="AB12" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="6"/>
-      <c r="V13" s="6"/>
-      <c r="W13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="X13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA13" s="6"/>
-      <c r="AB13" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
-      <c r="X14" s="2"/>
-      <c r="Y14" s="2"/>
-      <c r="Z14" s="2"/>
-      <c r="AB14" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
-      <c r="X15" s="2"/>
-      <c r="Y15" s="2"/>
-      <c r="Z15" s="2"/>
-      <c r="AA15" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC15" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-      <c r="X16" s="2"/>
-      <c r="Y16" s="2"/>
-      <c r="Z16" s="2"/>
-      <c r="AA16" s="2"/>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
-      <c r="X17" s="2"/>
-      <c r="Y17" s="2"/>
-      <c r="Z17" s="2"/>
-      <c r="AA17" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="L1:AA1"/>
-    <mergeCell ref="A3:A14"/>
-    <mergeCell ref="A16:A17"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DF78EAC-8188-4FCB-BF9A-2F2ECCDC7D75}">
-  <dimension ref="A1:BW16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U30" sqref="U30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
-    <col min="3" max="75" width="3.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="M1" s="12"/>
       <c r="N1" s="12"/>
       <c r="O1" s="12"/>
       <c r="P1" s="12"/>
@@ -1779,52 +951,994 @@
       <c r="AB1" s="12"/>
       <c r="AC1" s="12"/>
       <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="12"/>
-      <c r="AL1" s="12"/>
-      <c r="AM1" s="14"/>
-      <c r="AN1" s="14"/>
-      <c r="AO1" s="14"/>
-      <c r="AP1" s="14"/>
-      <c r="AQ1" s="14"/>
-      <c r="AR1" s="14"/>
-      <c r="AS1" s="14"/>
-      <c r="AT1" s="14"/>
-      <c r="AU1" s="14"/>
-      <c r="AV1" s="14"/>
-      <c r="AW1" s="14"/>
-      <c r="AX1" s="14"/>
-      <c r="AY1" s="14"/>
-      <c r="AZ1" s="14"/>
-      <c r="BB1" s="12"/>
-      <c r="BC1" s="12"/>
-      <c r="BD1" s="12"/>
-      <c r="BE1" s="12"/>
-      <c r="BF1" s="12"/>
-      <c r="BG1" s="12"/>
-      <c r="BH1" s="12"/>
-      <c r="BI1" s="12"/>
-      <c r="BJ1" s="12"/>
-      <c r="BK1" s="12"/>
-      <c r="BL1" s="14"/>
-      <c r="BM1" s="14"/>
-      <c r="BN1" s="14"/>
-      <c r="BO1" s="14"/>
-      <c r="BP1" s="14"/>
-      <c r="BQ1" s="14"/>
-      <c r="BR1" s="14"/>
-      <c r="BS1" s="14"/>
-      <c r="BT1" s="14"/>
-      <c r="BU1" s="14"/>
-      <c r="BV1" s="14"/>
-      <c r="BW1" s="14"/>
     </row>
-    <row r="2" spans="1:75" ht="219" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="159" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="V2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="W2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="X2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB2" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC2" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD2" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="15">
+        <v>1</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="18"/>
+      <c r="AA3" s="18"/>
+      <c r="AB3" s="19"/>
+      <c r="AC3" s="19"/>
+      <c r="AD3" s="18"/>
+    </row>
+    <row r="4" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="14"/>
+      <c r="B4" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="18"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="18"/>
+      <c r="Y4" s="18"/>
+      <c r="Z4" s="18"/>
+      <c r="AA4" s="18"/>
+      <c r="AB4" s="19"/>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="18"/>
+    </row>
+    <row r="5" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="14"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="23"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="18"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="18"/>
+      <c r="AB5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC5" s="19"/>
+      <c r="AD5" s="18"/>
+    </row>
+    <row r="6" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="14"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" s="23"/>
+      <c r="N6" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="18"/>
+      <c r="AA6" s="18"/>
+      <c r="AB6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC6" s="19"/>
+      <c r="AD6" s="18"/>
+    </row>
+    <row r="7" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="14"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="18"/>
+      <c r="V7" s="18"/>
+      <c r="W7" s="18"/>
+      <c r="X7" s="18"/>
+      <c r="Y7" s="18"/>
+      <c r="Z7" s="18"/>
+      <c r="AA7" s="18"/>
+      <c r="AB7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC7" s="19"/>
+      <c r="AD7" s="18"/>
+    </row>
+    <row r="8" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="14"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="18"/>
+      <c r="V8" s="18"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="18"/>
+      <c r="AA8" s="18"/>
+      <c r="AB8" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC8" s="19"/>
+      <c r="AD8" s="18"/>
+    </row>
+    <row r="9" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="14"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="18"/>
+      <c r="W9" s="18"/>
+      <c r="X9" s="18"/>
+      <c r="Y9" s="18"/>
+      <c r="Z9" s="18"/>
+      <c r="AA9" s="18"/>
+      <c r="AB9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC9" s="19"/>
+      <c r="AD9" s="18"/>
+    </row>
+    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="14"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="18"/>
+      <c r="W10" s="18"/>
+      <c r="X10" s="18"/>
+      <c r="Y10" s="18"/>
+      <c r="Z10" s="18"/>
+      <c r="AA10" s="18"/>
+      <c r="AB10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC10" s="19"/>
+      <c r="AD10" s="18"/>
+    </row>
+    <row r="11" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="14"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="L11" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="18"/>
+      <c r="T11" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="U11" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="V11" s="18"/>
+      <c r="W11" s="18"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="18"/>
+      <c r="Z11" s="18"/>
+      <c r="AA11" s="18"/>
+      <c r="AB11" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC11" s="19"/>
+      <c r="AD11" s="18"/>
+    </row>
+    <row r="12" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="14"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="18"/>
+      <c r="T12" s="24"/>
+      <c r="U12" s="24"/>
+      <c r="V12" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="W12" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="X12" s="18"/>
+      <c r="Y12" s="18"/>
+      <c r="Z12" s="18"/>
+      <c r="AA12" s="18"/>
+      <c r="AB12" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC12" s="19"/>
+      <c r="AD12" s="18"/>
+    </row>
+    <row r="13" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="14"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="18"/>
+      <c r="T13" s="24"/>
+      <c r="U13" s="24"/>
+      <c r="V13" s="18"/>
+      <c r="W13" s="18"/>
+      <c r="X13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC13" s="19"/>
+      <c r="AD13" s="18"/>
+    </row>
+    <row r="14" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="14"/>
+      <c r="B14" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="L14" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
+      <c r="T14" s="25"/>
+      <c r="U14" s="25"/>
+      <c r="V14" s="25"/>
+      <c r="W14" s="25"/>
+      <c r="X14" s="25"/>
+      <c r="Y14" s="25"/>
+      <c r="Z14" s="25"/>
+      <c r="AA14" s="25"/>
+      <c r="AB14" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC14" s="19"/>
+      <c r="AD14" s="19"/>
+    </row>
+    <row r="15" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="14"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
+      <c r="T15" s="25"/>
+      <c r="U15" s="25"/>
+      <c r="V15" s="25"/>
+      <c r="W15" s="25"/>
+      <c r="X15" s="25"/>
+      <c r="Y15" s="25"/>
+      <c r="Z15" s="25"/>
+      <c r="AA15" s="25"/>
+      <c r="AB15" s="19"/>
+      <c r="AC15" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD15" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="26"/>
+      <c r="C16" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
+      <c r="T16" s="25"/>
+      <c r="U16" s="25"/>
+      <c r="V16" s="25"/>
+      <c r="W16" s="25"/>
+      <c r="X16" s="25"/>
+      <c r="Y16" s="25"/>
+      <c r="Z16" s="25"/>
+      <c r="AA16" s="25"/>
+      <c r="AB16" s="19"/>
+      <c r="AC16" s="19"/>
+      <c r="AD16" s="25"/>
+    </row>
+    <row r="17" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="14"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="25"/>
+      <c r="V17" s="25"/>
+      <c r="W17" s="25"/>
+      <c r="X17" s="25"/>
+      <c r="Y17" s="25"/>
+      <c r="Z17" s="25"/>
+      <c r="AA17" s="25"/>
+      <c r="AB17" s="19"/>
+      <c r="AC17" s="19"/>
+      <c r="AD17" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="M1:AD1"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B4:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A3:A15"/>
+    <mergeCell ref="A1:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DF78EAC-8188-4FCB-BF9A-2F2ECCDC7D75}">
+  <dimension ref="A1:BW16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U30" sqref="U30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.7265625" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" customWidth="1"/>
+    <col min="3" max="75" width="3.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="8"/>
+      <c r="AM1" s="10"/>
+      <c r="AN1" s="10"/>
+      <c r="AO1" s="10"/>
+      <c r="AP1" s="10"/>
+      <c r="AQ1" s="10"/>
+      <c r="AR1" s="10"/>
+      <c r="AS1" s="10"/>
+      <c r="AT1" s="10"/>
+      <c r="AU1" s="10"/>
+      <c r="AV1" s="10"/>
+      <c r="AW1" s="10"/>
+      <c r="AX1" s="10"/>
+      <c r="AY1" s="10"/>
+      <c r="AZ1" s="10"/>
+      <c r="BB1" s="8"/>
+      <c r="BC1" s="8"/>
+      <c r="BD1" s="8"/>
+      <c r="BE1" s="8"/>
+      <c r="BF1" s="8"/>
+      <c r="BG1" s="8"/>
+      <c r="BH1" s="8"/>
+      <c r="BI1" s="8"/>
+      <c r="BJ1" s="8"/>
+      <c r="BK1" s="8"/>
+      <c r="BL1" s="10"/>
+      <c r="BM1" s="10"/>
+      <c r="BN1" s="10"/>
+      <c r="BO1" s="10"/>
+      <c r="BP1" s="10"/>
+      <c r="BQ1" s="10"/>
+      <c r="BR1" s="10"/>
+      <c r="BS1" s="10"/>
+      <c r="BT1" s="10"/>
+      <c r="BU1" s="10"/>
+      <c r="BV1" s="10"/>
+      <c r="BW1" s="10"/>
+    </row>
+    <row r="2" spans="1:75" ht="213" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>41</v>
@@ -2009,8 +2123,8 @@
       <c r="BV2" s="4"/>
       <c r="BW2" s="4"/>
     </row>
-    <row r="3" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -2118,8 +2232,8 @@
       <c r="BV3" s="6"/>
       <c r="BW3" s="6"/>
     </row>
-    <row r="4" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
+    <row r="4" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A4" s="9"/>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2233,8 +2347,8 @@
       <c r="BV4" s="5"/>
       <c r="BW4" s="5"/>
     </row>
-    <row r="5" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+    <row r="5" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A5" s="9"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2354,8 +2468,8 @@
       <c r="BV5" s="5"/>
       <c r="BW5" s="5"/>
     </row>
-    <row r="6" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+    <row r="6" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A6" s="9"/>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2475,8 +2589,8 @@
       <c r="BV6" s="5"/>
       <c r="BW6" s="5"/>
     </row>
-    <row r="7" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
+    <row r="7" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A7" s="9"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2598,8 +2712,8 @@
       <c r="BV7" s="5"/>
       <c r="BW7" s="5"/>
     </row>
-    <row r="8" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
+    <row r="8" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A8" s="9"/>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2723,8 +2837,8 @@
       <c r="BV8" s="5"/>
       <c r="BW8" s="5"/>
     </row>
-    <row r="9" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
+    <row r="9" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A9" s="9"/>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2840,8 +2954,8 @@
       <c r="BV9" s="5"/>
       <c r="BW9" s="5"/>
     </row>
-    <row r="10" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
+    <row r="10" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A10" s="9"/>
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2961,8 +3075,8 @@
       <c r="BV10" s="5"/>
       <c r="BW10" s="5"/>
     </row>
-    <row r="11" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
+    <row r="11" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A11" s="9"/>
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
@@ -3088,8 +3202,8 @@
       <c r="BV11" s="5"/>
       <c r="BW11" s="5"/>
     </row>
-    <row r="12" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
+    <row r="12" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A12" s="9"/>
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
@@ -3207,8 +3321,8 @@
       <c r="BV12" s="5"/>
       <c r="BW12" s="5"/>
     </row>
-    <row r="13" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
+    <row r="13" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A13" s="9"/>
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
@@ -3330,8 +3444,8 @@
       <c r="BV13" s="5"/>
       <c r="BW13" s="5"/>
     </row>
-    <row r="14" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
+    <row r="14" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A14" s="9"/>
       <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
@@ -3437,7 +3551,7 @@
       <c r="BV14" s="5"/>
       <c r="BW14" s="5"/>
     </row>
-    <row r="15" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
         <v>38</v>
@@ -3516,7 +3630,7 @@
       <c r="BV15" s="2"/>
       <c r="BW15" s="2"/>
     </row>
-    <row r="16" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="1" t="s">
         <v>39</v>

</xml_diff>